<commit_message>
Board and BOM update
</commit_message>
<xml_diff>
--- a/- PCB -/QRE MiniBoards/QRE MiniBoards BOM.xlsx
+++ b/- PCB -/QRE MiniBoards/QRE MiniBoards BOM.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\RoboCop\- PCB -\QRE MiniBoards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E90028EC-9F78-4522-B9E1-A349D59C9F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CF1E35-B290-4C57-B71A-5D9C3E325DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QRE MiniBoards" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -82,7 +95,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -716,9 +729,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 –⁠ 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -756,7 +769,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 –⁠ 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -862,7 +875,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 –⁠ 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1004,24 +1017,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="29.36328125" customWidth="1"/>
-    <col min="3" max="3" width="50.453125" customWidth="1"/>
+    <col min="3" max="3" width="55.54296875" customWidth="1"/>
     <col min="4" max="4" width="6.6328125" customWidth="1"/>
     <col min="5" max="5" width="21.90625" customWidth="1"/>
     <col min="6" max="6" width="16.36328125" customWidth="1"/>
@@ -1137,6 +1150,12 @@
       </c>
       <c r="F6" s="1"/>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <f>SUM(D2:D7)</f>
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>